<commit_message>
add scann qrcode page
</commit_message>
<xml_diff>
--- a/public/assets/template/sampleImportAset.xlsx
+++ b/public/assets/template/sampleImportAset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\manajemen-aset\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D51981FB-24A4-4259-97B0-B08E4D247DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD83457-C039-4235-9C9F-032AE6F584DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{DC3E753A-C2FB-473A-BBF8-4BCBA285966F}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>Kode Ruang</t>
   </si>
   <si>
-    <t>Uraian Ruang</t>
-  </si>
-  <si>
     <t>Catatan</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>Sumber Pengadaan</t>
+  </si>
+  <si>
+    <t>Kode Gedung</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,25 +525,25 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>